<commit_message>
Sala Covid Semana 48
</commit_message>
<xml_diff>
--- a/tablas/tabla_defunciones_cero.xlsx
+++ b/tablas/tabla_defunciones_cero.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\GERESA_covid_cusco\tablas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\GERESA_covid_cusco\tablas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06983FC9-4DE6-4851-B366-455F3A3820A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDECDD1-22FD-45C2-9CEB-13E88A6451B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B35F084E-A87D-4054-80F3-C51BCACE92B8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B35F084E-A87D-4054-80F3-C51BCACE92B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -197,7 +197,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -214,11 +214,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -242,6 +260,25 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{994E6999-8BCD-4B3C-B1C7-C4CF1750CA02}">
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,7 +611,7 @@
     <col min="3" max="6" width="11.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -591,7 +628,7 @@
       <c r="N1" s="10"/>
       <c r="O1" s="10"/>
     </row>
-    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="7" t="s">
         <v>17</v>
@@ -636,7 +673,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="8" t="s">
         <v>16</v>
@@ -681,7 +718,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -692,17 +729,20 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -715,19 +755,24 @@
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="4">
-        <v>1</v>
-      </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G5" s="14">
+        <v>1</v>
+      </c>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="14">
+        <v>6</v>
+      </c>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -738,17 +783,22 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="14">
+        <v>4</v>
+      </c>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -761,21 +811,26 @@
         <v>1</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="4">
-        <v>1</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="4">
-        <v>1</v>
-      </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G7" s="14">
+        <v>1</v>
+      </c>
+      <c r="H7" s="15"/>
+      <c r="I7" s="14">
+        <v>1</v>
+      </c>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="14">
+        <v>1</v>
+      </c>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -788,19 +843,24 @@
       <c r="F8" s="4">
         <v>2</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="4">
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="14">
         <v>2</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="14">
+        <v>4</v>
+      </c>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -813,27 +873,32 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="4">
-        <v>1</v>
-      </c>
-      <c r="H9" s="4">
-        <v>1</v>
-      </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="4">
-        <v>1</v>
-      </c>
-      <c r="K9" s="4">
-        <v>1</v>
-      </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="4">
-        <v>1</v>
-      </c>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G9" s="14">
+        <v>1</v>
+      </c>
+      <c r="H9" s="14">
+        <v>1</v>
+      </c>
+      <c r="I9" s="15"/>
+      <c r="J9" s="14">
+        <v>1</v>
+      </c>
+      <c r="K9" s="14">
+        <v>1</v>
+      </c>
+      <c r="L9" s="15"/>
+      <c r="M9" s="14">
+        <v>1</v>
+      </c>
+      <c r="N9" s="15"/>
+      <c r="O9" s="14">
+        <v>2</v>
+      </c>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="12"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -852,27 +917,32 @@
       <c r="F10" s="4">
         <v>3</v>
       </c>
-      <c r="G10" s="4">
-        <v>1</v>
-      </c>
-      <c r="H10" s="4">
+      <c r="G10" s="14">
+        <v>1</v>
+      </c>
+      <c r="H10" s="14">
         <v>4</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="14">
         <v>3</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="14">
         <v>2</v>
       </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="4">
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="14">
         <v>2</v>
       </c>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N10" s="15"/>
+      <c r="O10" s="14">
+        <v>12</v>
+      </c>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -883,17 +953,22 @@
       <c r="F11" s="4">
         <v>1</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="14">
+        <v>2</v>
+      </c>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -910,21 +985,26 @@
       <c r="F12" s="4">
         <v>1</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="14">
         <v>2</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="4">
-        <v>1</v>
-      </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="14">
+        <v>1</v>
+      </c>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="14">
+        <v>4</v>
+      </c>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -935,19 +1015,24 @@
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="4">
-        <v>1</v>
-      </c>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="14">
+        <v>1</v>
+      </c>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="14">
+        <v>2</v>
+      </c>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -956,21 +1041,24 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="4">
-        <v>1</v>
-      </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="4">
-        <v>1</v>
-      </c>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G14" s="14">
+        <v>1</v>
+      </c>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="14">
+        <v>1</v>
+      </c>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -981,19 +1069,24 @@
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="4">
-        <v>1</v>
-      </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G15" s="15"/>
+      <c r="H15" s="14">
+        <v>1</v>
+      </c>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="14">
+        <v>7</v>
+      </c>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+    </row>
+    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>12</v>
       </c>
@@ -1006,17 +1099,27 @@
       <c r="F16" s="6">
         <v>1</v>
       </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="6">
-        <v>1</v>
-      </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="17">
+        <v>1</v>
+      </c>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="17">
+        <v>4</v>
+      </c>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+    </row>
+    <row r="17" spans="16:18" x14ac:dyDescent="0.25">
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
SALA SITUACIONAL SEM 49
</commit_message>
<xml_diff>
--- a/tablas/tabla_defunciones_cero.xlsx
+++ b/tablas/tabla_defunciones_cero.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\GERESA_covid_cusco\tablas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC624F8-F131-45BF-8CD9-61D5F398EBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542F0E4E-9ADB-4B53-846B-36926D142B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B35F084E-A87D-4054-80F3-C51BCACE92B8}"/>
   </bookViews>
@@ -607,7 +607,7 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,7 +950,9 @@
       <c r="O10" s="14">
         <v>1</v>
       </c>
-      <c r="P10" s="15"/>
+      <c r="P10" s="14">
+        <v>1</v>
+      </c>
       <c r="Q10" s="12"/>
       <c r="R10" s="12"/>
       <c r="S10" s="12"/>

</xml_diff>

<commit_message>
Revert "SALA SITUACIONAL SEM 49"
This reverts commit f3add1c3a71705fdd1d7bb15b9fc80d3de7a3205.
</commit_message>
<xml_diff>
--- a/tablas/tabla_defunciones_cero.xlsx
+++ b/tablas/tabla_defunciones_cero.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\GERESA_covid_cusco\tablas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542F0E4E-9ADB-4B53-846B-36926D142B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC624F8-F131-45BF-8CD9-61D5F398EBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B35F084E-A87D-4054-80F3-C51BCACE92B8}"/>
   </bookViews>
@@ -607,7 +607,7 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,9 +950,7 @@
       <c r="O10" s="14">
         <v>1</v>
       </c>
-      <c r="P10" s="14">
-        <v>1</v>
-      </c>
+      <c r="P10" s="15"/>
       <c r="Q10" s="12"/>
       <c r="R10" s="12"/>
       <c r="S10" s="12"/>

</xml_diff>

<commit_message>
Sala Situacional Sem 10
</commit_message>
<xml_diff>
--- a/tablas/tabla_defunciones_cero.xlsx
+++ b/tablas/tabla_defunciones_cero.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\GERESA_covid_cusco\tablas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEI-02\Documents\GitHub\GERESA_covid_cusco\tablas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D29C2A1-2A97-4A4F-A9D9-37B265345D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F91460-2F50-4E3F-A6FB-0AAC9C67A947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B35F084E-A87D-4054-80F3-C51BCACE92B8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
   <si>
     <t>Acomayo</t>
   </si>
@@ -232,6 +232,12 @@
   </si>
   <si>
     <t>27feb-05mar</t>
+  </si>
+  <si>
+    <t>06mar-12mar</t>
+  </si>
+  <si>
+    <t>SE-10</t>
   </si>
 </sst>
 </file>
@@ -723,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{994E6999-8BCD-4B3C-B1C7-C4CF1750CA02}">
-  <dimension ref="A1:AE17"/>
+  <dimension ref="A1:AF17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB15" sqref="AB15"/>
+      <selection activeCell="AD10" sqref="AD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,7 +743,7 @@
     <col min="7" max="17" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -766,8 +772,9 @@
       <c r="Z1" s="10"/>
       <c r="AA1" s="10"/>
       <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
     </row>
-    <row r="2" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="7" t="s">
         <v>17</v>
@@ -850,8 +857,11 @@
       <c r="AB2" s="7" t="s">
         <v>64</v>
       </c>
+      <c r="AC2" s="7" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="3" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="8" t="s">
         <v>16</v>
@@ -934,8 +944,11 @@
       <c r="AB3" s="8" t="s">
         <v>65</v>
       </c>
+      <c r="AC3" s="8" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -970,10 +983,11 @@
         <v>1</v>
       </c>
       <c r="AB4" s="18"/>
-      <c r="AC4" s="12"/>
+      <c r="AC4" s="18"/>
       <c r="AD4" s="12"/>
+      <c r="AE4" s="12"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1018,10 +1032,13 @@
       </c>
       <c r="AA5" s="18"/>
       <c r="AB5" s="18"/>
-      <c r="AC5" s="12"/>
+      <c r="AC5" s="24">
+        <v>1</v>
+      </c>
       <c r="AD5" s="12"/>
+      <c r="AE5" s="12"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1064,10 +1081,13 @@
         <v>1</v>
       </c>
       <c r="AB6" s="18"/>
-      <c r="AC6" s="12"/>
+      <c r="AC6" s="24">
+        <v>1</v>
+      </c>
       <c r="AD6" s="12"/>
+      <c r="AE6" s="12"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1112,10 +1132,11 @@
       </c>
       <c r="AA7" s="18"/>
       <c r="AB7" s="18"/>
-      <c r="AC7" s="12"/>
+      <c r="AC7" s="18"/>
       <c r="AD7" s="12"/>
+      <c r="AE7" s="12"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1172,11 +1193,14 @@
         <v>1</v>
       </c>
       <c r="AB8" s="18"/>
-      <c r="AC8" s="22"/>
-      <c r="AD8" s="21"/>
-      <c r="AE8" s="23"/>
+      <c r="AC8" s="24">
+        <v>3</v>
+      </c>
+      <c r="AD8" s="22"/>
+      <c r="AE8" s="21"/>
+      <c r="AF8" s="23"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1231,11 +1255,12 @@
       </c>
       <c r="AA9" s="18"/>
       <c r="AB9" s="18"/>
-      <c r="AC9" s="11"/>
-      <c r="AD9" s="21"/>
-      <c r="AE9" s="23"/>
+      <c r="AC9" s="18"/>
+      <c r="AD9" s="11"/>
+      <c r="AE9" s="21"/>
+      <c r="AF9" s="23"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1308,11 +1333,14 @@
       <c r="AB10" s="24">
         <v>1</v>
       </c>
-      <c r="AC10" s="22"/>
-      <c r="AD10" s="21"/>
-      <c r="AE10" s="23"/>
+      <c r="AC10" s="24">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="22"/>
+      <c r="AE10" s="21"/>
+      <c r="AF10" s="23"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1359,11 +1387,12 @@
         <v>2</v>
       </c>
       <c r="AB11" s="18"/>
-      <c r="AC11" s="22"/>
-      <c r="AD11" s="21"/>
-      <c r="AE11" s="23"/>
+      <c r="AC11" s="18"/>
+      <c r="AD11" s="22"/>
+      <c r="AE11" s="21"/>
+      <c r="AF11" s="23"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1424,11 +1453,14 @@
       <c r="AB12" s="24">
         <v>1</v>
       </c>
-      <c r="AC12" s="22"/>
-      <c r="AD12" s="21"/>
-      <c r="AE12" s="23"/>
+      <c r="AC12" s="24">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="22"/>
+      <c r="AE12" s="21"/>
+      <c r="AF12" s="23"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1471,11 +1503,12 @@
       <c r="AB13" s="24">
         <v>1</v>
       </c>
-      <c r="AC13" s="12"/>
-      <c r="AD13" s="21"/>
-      <c r="AE13" s="23"/>
+      <c r="AC13" s="18"/>
+      <c r="AD13" s="12"/>
+      <c r="AE13" s="21"/>
+      <c r="AF13" s="23"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1518,11 +1551,14 @@
       <c r="Z14" s="18"/>
       <c r="AA14" s="18"/>
       <c r="AB14" s="18"/>
-      <c r="AC14" s="22"/>
-      <c r="AD14" s="21"/>
-      <c r="AE14" s="23"/>
+      <c r="AC14" s="24">
+        <v>1</v>
+      </c>
+      <c r="AD14" s="22"/>
+      <c r="AE14" s="21"/>
+      <c r="AF14" s="23"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -1569,10 +1605,11 @@
       <c r="AB15" s="24">
         <v>1</v>
       </c>
-      <c r="AC15" s="12"/>
+      <c r="AC15" s="18"/>
       <c r="AD15" s="12"/>
+      <c r="AE15" s="12"/>
     </row>
-    <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>12</v>
       </c>
@@ -1619,12 +1656,13 @@
         <v>2</v>
       </c>
       <c r="AB16" s="18"/>
-      <c r="AC16" s="21"/>
-      <c r="AD16" s="12"/>
+      <c r="AC16" s="18"/>
+      <c r="AD16" s="21"/>
+      <c r="AE16" s="12"/>
     </row>
-    <row r="17" spans="29:30" x14ac:dyDescent="0.25">
-      <c r="AC17" s="12"/>
+    <row r="17" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD17" s="12"/>
+      <c r="AE17" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Actualizando Sala Sem 12
</commit_message>
<xml_diff>
--- a/tablas/tabla_defunciones_cero.xlsx
+++ b/tablas/tabla_defunciones_cero.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEI-02\Documents\GitHub\GERESA_covid_cusco\tablas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\GERESA_covid_cusco\tablas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9599F993-EEA9-48A6-88A9-80E6AE4038F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF7C24A-C834-4111-8AEE-5FB22B3FDC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B35F084E-A87D-4054-80F3-C51BCACE92B8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
   <si>
     <t>Acomayo</t>
   </si>
@@ -244,6 +244,12 @@
   </si>
   <si>
     <t>13mar-19mar</t>
+  </si>
+  <si>
+    <t>SE-12</t>
+  </si>
+  <si>
+    <t>20mar-26mar</t>
   </si>
 </sst>
 </file>
@@ -735,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{994E6999-8BCD-4B3C-B1C7-C4CF1750CA02}">
-  <dimension ref="A1:AG17"/>
+  <dimension ref="A1:AH17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+      <selection activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,10 +752,10 @@
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" hidden="1" customWidth="1"/>
     <col min="3" max="6" width="11.140625" hidden="1" customWidth="1"/>
-    <col min="7" max="21" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="22" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -780,8 +786,9 @@
       <c r="AB1" s="10"/>
       <c r="AC1" s="10"/>
       <c r="AD1" s="10"/>
+      <c r="AE1" s="10"/>
     </row>
-    <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="7" t="s">
         <v>17</v>
@@ -870,8 +877,11 @@
       <c r="AD2" s="7" t="s">
         <v>68</v>
       </c>
+      <c r="AE2" s="7" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="3" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="8" t="s">
         <v>16</v>
@@ -960,8 +970,11 @@
       <c r="AD3" s="8" t="s">
         <v>69</v>
       </c>
+      <c r="AE3" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -998,10 +1011,11 @@
       <c r="AB4" s="18"/>
       <c r="AC4" s="18"/>
       <c r="AD4" s="18"/>
-      <c r="AE4" s="12"/>
+      <c r="AE4" s="18"/>
       <c r="AF4" s="12"/>
+      <c r="AG4" s="12"/>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1050,10 +1064,11 @@
         <v>1</v>
       </c>
       <c r="AD5" s="18"/>
-      <c r="AE5" s="12"/>
+      <c r="AE5" s="18"/>
       <c r="AF5" s="12"/>
+      <c r="AG5" s="12"/>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1102,10 +1117,11 @@
       <c r="AD6" s="24">
         <v>1</v>
       </c>
-      <c r="AE6" s="12"/>
+      <c r="AE6" s="18"/>
       <c r="AF6" s="12"/>
+      <c r="AG6" s="12"/>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1152,10 +1168,11 @@
       <c r="AB7" s="18"/>
       <c r="AC7" s="18"/>
       <c r="AD7" s="18"/>
-      <c r="AE7" s="12"/>
+      <c r="AE7" s="18"/>
       <c r="AF7" s="12"/>
+      <c r="AG7" s="12"/>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1218,11 +1235,12 @@
       <c r="AD8" s="24">
         <v>1</v>
       </c>
-      <c r="AE8" s="22"/>
-      <c r="AF8" s="21"/>
-      <c r="AG8" s="23"/>
+      <c r="AE8" s="18"/>
+      <c r="AF8" s="22"/>
+      <c r="AG8" s="21"/>
+      <c r="AH8" s="23"/>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1281,11 +1299,12 @@
       <c r="AD9" s="24">
         <v>1</v>
       </c>
-      <c r="AE9" s="11"/>
-      <c r="AF9" s="21"/>
-      <c r="AG9" s="23"/>
+      <c r="AE9" s="18"/>
+      <c r="AF9" s="11"/>
+      <c r="AG9" s="21"/>
+      <c r="AH9" s="23"/>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1364,11 +1383,14 @@
       <c r="AD10" s="24">
         <v>1</v>
       </c>
-      <c r="AE10" s="22"/>
-      <c r="AF10" s="21"/>
-      <c r="AG10" s="23"/>
+      <c r="AE10" s="24">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="22"/>
+      <c r="AG10" s="21"/>
+      <c r="AH10" s="23"/>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1417,11 +1439,12 @@
       <c r="AB11" s="18"/>
       <c r="AC11" s="18"/>
       <c r="AD11" s="18"/>
-      <c r="AE11" s="22"/>
-      <c r="AF11" s="21"/>
-      <c r="AG11" s="23"/>
+      <c r="AE11" s="18"/>
+      <c r="AF11" s="22"/>
+      <c r="AG11" s="21"/>
+      <c r="AH11" s="23"/>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1486,11 +1509,14 @@
         <v>1</v>
       </c>
       <c r="AD12" s="18"/>
-      <c r="AE12" s="22"/>
-      <c r="AF12" s="21"/>
-      <c r="AG12" s="23"/>
+      <c r="AE12" s="24">
+        <v>1</v>
+      </c>
+      <c r="AF12" s="22"/>
+      <c r="AG12" s="21"/>
+      <c r="AH12" s="23"/>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1535,11 +1561,12 @@
       </c>
       <c r="AC13" s="18"/>
       <c r="AD13" s="18"/>
-      <c r="AE13" s="12"/>
-      <c r="AF13" s="21"/>
-      <c r="AG13" s="23"/>
+      <c r="AE13" s="18"/>
+      <c r="AF13" s="12"/>
+      <c r="AG13" s="21"/>
+      <c r="AH13" s="23"/>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1586,11 +1613,12 @@
         <v>1</v>
       </c>
       <c r="AD14" s="18"/>
-      <c r="AE14" s="22"/>
-      <c r="AF14" s="21"/>
-      <c r="AG14" s="23"/>
+      <c r="AE14" s="18"/>
+      <c r="AF14" s="22"/>
+      <c r="AG14" s="21"/>
+      <c r="AH14" s="23"/>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -1639,10 +1667,11 @@
       </c>
       <c r="AC15" s="18"/>
       <c r="AD15" s="18"/>
-      <c r="AE15" s="12"/>
+      <c r="AE15" s="18"/>
       <c r="AF15" s="12"/>
+      <c r="AG15" s="12"/>
     </row>
-    <row r="16" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>12</v>
       </c>
@@ -1691,12 +1720,13 @@
       <c r="AB16" s="18"/>
       <c r="AC16" s="18"/>
       <c r="AD16" s="18"/>
-      <c r="AE16" s="21"/>
-      <c r="AF16" s="12"/>
+      <c r="AE16" s="18"/>
+      <c r="AF16" s="21"/>
+      <c r="AG16" s="12"/>
     </row>
-    <row r="17" spans="31:32" x14ac:dyDescent="0.25">
-      <c r="AE17" s="12"/>
+    <row r="17" spans="32:33" x14ac:dyDescent="0.25">
       <c r="AF17" s="12"/>
+      <c r="AG17" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>